<commit_message>
IND OTH still has a couple calibration issues
A few small issues on electricity consumption for a couple techs. But I think can only be solved once in full model and updated supply model sectors.
</commit_message>
<xml_diff>
--- a/vt_REGION1_IND-OTH.xlsx
+++ b/vt_REGION1_IND-OTH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AADA38-1D33-40E1-966B-6ED8BE62D21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DB8599-64D9-4BAB-8297-F5846C63437E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="853" activeTab="9" xr2:uid="{43DCB660-3C9F-4D21-841F-0AAFE0E93A09}"/>
+    <workbookView xWindow="10905" yWindow="225" windowWidth="20625" windowHeight="15435" tabRatio="853" activeTab="9" xr2:uid="{43DCB660-3C9F-4D21-841F-0AAFE0E93A09}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="99" r:id="rId1"/>
@@ -1786,7 +1786,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3231" uniqueCount="836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3231" uniqueCount="837">
   <si>
     <t>TimeSlice Version</t>
   </si>
@@ -4400,6 +4400,9 @@
   </si>
   <si>
     <t>~FI_T</t>
+  </si>
+  <si>
+    <t>INDGMU</t>
   </si>
 </sst>
 </file>
@@ -14893,20 +14896,19 @@
       <sheetName val="HDRI scenarios"/>
       <sheetName val="H-DRI literature and calcs"/>
       <sheetName val="Summary Hydrogen DRI new"/>
-      <sheetName val="Summary Hydrogen DRI"/>
-      <sheetName val="HDRI-Items"/>
       <sheetName val="HDRI-TSData"/>
       <sheetName val="HDRI-TIDData"/>
       <sheetName val="IS-Items"/>
       <sheetName val="IS-TSData"/>
       <sheetName val="IS-TIDData"/>
       <sheetName val="Iron &amp; Steel"/>
+      <sheetName val="veda Process def"/>
       <sheetName val="I&amp;S SATIM input"/>
       <sheetName val="Energy Intensity"/>
-      <sheetName val="I&amp;S capacity + production"/>
+      <sheetName val="Methodology Cap &amp; Prod"/>
+      <sheetName val="Coke"/>
       <sheetName val="Energy and Emissions"/>
       <sheetName val="Scrap"/>
-      <sheetName val="Coke"/>
       <sheetName val="TNapp - Opex sheet"/>
       <sheetName val="TNapp - Capex sheet"/>
       <sheetName val="TNapp - I&amp;S intensity"/>
@@ -14917,6 +14919,9 @@
       <sheetName val="Blast furnace JPN info"/>
       <sheetName val="Vereeniging"/>
       <sheetName val="Evraz Highveld"/>
+      <sheetName val="HDRI-Items"/>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet2"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -14958,7 +14963,9 @@
       <sheetData sheetId="25"/>
       <sheetData sheetId="26"/>
       <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -14967,6 +14974,9 @@
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Log"/>
       <sheetName val="NameConv"/>
@@ -15004,20 +15014,19 @@
       <sheetName val="CommData"/>
       <sheetName val="ITEMS_Comm (jm)"/>
       <sheetName val="AFA"/>
-      <sheetName val="vt_REGION1_IND-NMM"/>
     </sheetNames>
     <definedNames>
       <definedName name="pamsindex" refersTo="='PAMS levers'!$C$3"/>
     </definedNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
       <sheetData sheetId="8">
         <row r="3">
           <cell r="C3" t="b">
@@ -15030,34 +15039,33 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -15972,8 +15980,8 @@
   </sheetPr>
   <dimension ref="A1:AY273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P137" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AW119" sqref="AW119"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="12.75"/>
@@ -24784,7 +24792,7 @@
         <v>ICPTGMU-E</v>
       </c>
       <c r="C124" s="213" t="s">
-        <v>470</v>
+        <v>836</v>
       </c>
       <c r="D124" s="46" t="str">
         <f>$B$5&amp;RIGHT($B103,2)&amp;$B$71</f>
@@ -41900,7 +41908,7 @@
       </c>
       <c r="H4" s="98">
         <f ca="1">NOW()</f>
-        <v>43698.705245717596</v>
+        <v>43707.464790046295</v>
       </c>
     </row>
     <row r="5" spans="1:8">

</xml_diff>

<commit_message>
mistake in elc boiler efficiency for mining fixed
</commit_message>
<xml_diff>
--- a/vt_REGION1_IND-OTH.xlsx
+++ b/vt_REGION1_IND-OTH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B466046-126A-41D7-95BD-3022024685D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1764753D-7C9C-4A77-9C55-F1EC4FF463FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="853" activeTab="9" xr2:uid="{43DCB660-3C9F-4D21-841F-0AAFE0E93A09}"/>
+    <workbookView xWindow="-5340" yWindow="-21720" windowWidth="38640" windowHeight="21240" tabRatio="853" activeTab="9" xr2:uid="{43DCB660-3C9F-4D21-841F-0AAFE0E93A09}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="99" r:id="rId1"/>
@@ -14989,15 +14989,15 @@
       <sheetName val="2017 inputs to SATIM"/>
       <sheetName val="NMM data"/>
       <sheetName val="Sheet1"/>
-      <sheetName val="Sheet2"/>
+      <sheetName val="INPUT - com defs"/>
+      <sheetName val="INPUT proc defs"/>
       <sheetName val="ClinkerSubstitution"/>
       <sheetName val="Cement Methodology"/>
-      <sheetName val="INPUT - com defs"/>
-      <sheetName val="INPUT proc defs"/>
       <sheetName val="INPUT - cement"/>
       <sheetName val="Bricks methodology"/>
       <sheetName val="Glass methodology"/>
       <sheetName val="Lime methodology"/>
+      <sheetName val="Sheet2"/>
       <sheetName val="INPUT - lime"/>
       <sheetName val="IND_NMM_2017_Dummy_processes "/>
       <sheetName val="ITEMS_Comm_Grp"/>
@@ -15051,10 +15051,10 @@
       <sheetData sheetId="19"/>
       <sheetData sheetId="20"/>
       <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
       <sheetData sheetId="26" refreshError="1"/>
       <sheetData sheetId="27" refreshError="1"/>
       <sheetData sheetId="28" refreshError="1"/>
@@ -15186,6 +15186,8 @@
       <sheetName val="ANSv2-692-ProcData"/>
       <sheetName val="ProcData_F_Mn_Cr - PAMS"/>
       <sheetName val="NetZero work"/>
+      <sheetName val="Chrome methodology"/>
+      <sheetName val="Sheet1"/>
       <sheetName val="Production and Capacity"/>
       <sheetName val="RES of chrome industry with EE"/>
       <sheetName val="ANSv2-692-ConstrData"/>
@@ -15196,7 +15198,6 @@
       <sheetName val="ANSv2-692-TS TRADE"/>
       <sheetName val="ANSv2-692-TID TRADE"/>
       <sheetName val="ANSv2-692-TS&amp;TID TRADE"/>
-      <sheetName val="vt_REGION1_IND-FA"/>
     </sheetNames>
     <definedNames>
       <definedName name="FA_PAMS_index" refersTo="='Index'!$J$5"/>
@@ -15242,7 +15243,8 @@
       <sheetData sheetId="26"/>
       <sheetData sheetId="27"/>
       <sheetData sheetId="28"/>
-      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -15978,8 +15980,8 @@
   </sheetPr>
   <dimension ref="A1:AY273"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="12.75"/>
@@ -21748,8 +21750,8 @@
         <v>IMIS</v>
       </c>
       <c r="E95" s="58">
-        <f>Methodology!C44</f>
-        <v>0.6</v>
+        <f>Methodology!C27</f>
+        <v>0.76</v>
       </c>
       <c r="F95" s="60">
         <f>SUMIF(AFA!$C$3:$L$3,RIGHT(D95,1),AFA!$C$4:$L$4)</f>
@@ -42176,7 +42178,7 @@
       </c>
       <c r="H4" s="98">
         <f ca="1">NOW()</f>
-        <v>43727.434962037034</v>
+        <v>43741.375756597219</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -46324,7 +46326,7 @@
   </sheetPr>
   <dimension ref="B1:AE103"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="J75" sqref="J75"/>
     </sheetView>
   </sheetViews>

</xml_diff>